<commit_message>
Konacna ispravka forme, liste rade i izbrisani su svi nebitni kometari.
</commit_message>
<xml_diff>
--- a/forme/templates/naruci.xlsx
+++ b/forme/templates/naruci.xlsx
@@ -324,117 +324,11 @@
   </cellStyleXfs>
   <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -442,6 +336,112 @@
     <xf numFmtId="165" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -725,7 +725,7 @@
   <dimension ref="A2:L23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E2" workbookViewId="0">
-      <selection activeCell="L23" sqref="L23"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -742,24 +742,24 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="2" t="s">
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="2"/>
+      <c r="G2" s="43"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
+      <c r="B3" s="42"/>
+      <c r="C3" s="42"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -773,177 +773,177 @@
       <c r="A6" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="5"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="29"/>
       <c r="G6" t="s">
         <v>9</v>
       </c>
-      <c r="H6" s="9" t="s">
+      <c r="H6" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
-      <c r="L6" s="11"/>
+      <c r="I6" s="34"/>
+      <c r="J6" s="34"/>
+      <c r="K6" s="34"/>
+      <c r="L6" s="35"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="5"/>
+      <c r="C7" s="28"/>
+      <c r="D7" s="29"/>
       <c r="G7" t="s">
         <v>10</v>
       </c>
-      <c r="H7" s="12" t="s">
+      <c r="H7" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="I7" s="13"/>
-      <c r="J7" s="13"/>
-      <c r="K7" s="13"/>
-      <c r="L7" s="14"/>
+      <c r="I7" s="37"/>
+      <c r="J7" s="37"/>
+      <c r="K7" s="37"/>
+      <c r="L7" s="38"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="5"/>
+      <c r="C8" s="28"/>
+      <c r="D8" s="29"/>
       <c r="G8" t="s">
         <v>11</v>
       </c>
-      <c r="H8" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="I8" s="13"/>
-      <c r="J8" s="13"/>
-      <c r="K8" s="13"/>
-      <c r="L8" s="14"/>
+      <c r="H8" s="36" t="s">
+        <v>19</v>
+      </c>
+      <c r="I8" s="37"/>
+      <c r="J8" s="37"/>
+      <c r="K8" s="37"/>
+      <c r="L8" s="38"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="5"/>
+      <c r="C9" s="28"/>
+      <c r="D9" s="29"/>
       <c r="G9" t="s">
         <v>12</v>
       </c>
-      <c r="H9" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="I9" s="13"/>
-      <c r="J9" s="13"/>
-      <c r="K9" s="13"/>
-      <c r="L9" s="14"/>
+      <c r="H9" s="36" t="s">
+        <v>20</v>
+      </c>
+      <c r="I9" s="37"/>
+      <c r="J9" s="37"/>
+      <c r="K9" s="37"/>
+      <c r="L9" s="38"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="4"/>
-      <c r="D10" s="5"/>
+      <c r="C10" s="28"/>
+      <c r="D10" s="29"/>
       <c r="G10" t="s">
         <v>13</v>
       </c>
-      <c r="H10" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="I10" s="13"/>
-      <c r="J10" s="13"/>
-      <c r="K10" s="13"/>
-      <c r="L10" s="14"/>
+      <c r="H10" s="39" t="s">
+        <v>21</v>
+      </c>
+      <c r="I10" s="40"/>
+      <c r="J10" s="40"/>
+      <c r="K10" s="40"/>
+      <c r="L10" s="41"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="7"/>
-      <c r="D11" s="8"/>
+      <c r="C11" s="31"/>
+      <c r="D11" s="32"/>
       <c r="G11" t="s">
         <v>14</v>
       </c>
-      <c r="H11" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="I11" s="16"/>
-      <c r="J11" s="16"/>
-      <c r="K11" s="16"/>
-      <c r="L11" s="17"/>
+      <c r="H11" s="39" t="s">
+        <v>18</v>
+      </c>
+      <c r="I11" s="40"/>
+      <c r="J11" s="40"/>
+      <c r="K11" s="40"/>
+      <c r="L11" s="41"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="18" t="s">
+      <c r="B15" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="19"/>
-      <c r="D15" s="20"/>
-      <c r="F15" s="27" t="s">
+      <c r="C15" s="10"/>
+      <c r="D15" s="11"/>
+      <c r="F15" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="G15" s="27"/>
-      <c r="H15" s="28"/>
-      <c r="I15" s="29" t="s">
+      <c r="G15" s="18"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="J15" s="29"/>
+      <c r="J15" s="19"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B16" s="21"/>
-      <c r="C16" s="22"/>
-      <c r="D16" s="23"/>
-      <c r="F16" s="30" t="s">
+      <c r="B16" s="12"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="14"/>
+      <c r="F16" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="G16" s="30"/>
-      <c r="H16" s="28"/>
-      <c r="I16" s="31" t="s">
+      <c r="G16" s="20"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="J16" s="32"/>
-      <c r="L16" s="43" t="s">
+      <c r="J16" s="22"/>
+      <c r="L16" s="8" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B17" s="24"/>
-      <c r="C17" s="25"/>
-      <c r="D17" s="26"/>
-      <c r="F17" s="30"/>
-      <c r="G17" s="30"/>
-      <c r="H17" s="28"/>
-      <c r="I17" s="33"/>
-      <c r="J17" s="34"/>
-      <c r="L17" s="43" t="s">
+      <c r="B17" s="15"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="17"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="20"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="23"/>
+      <c r="J17" s="24"/>
+      <c r="L17" s="8" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="F18" s="30"/>
-      <c r="G18" s="30"/>
-      <c r="H18" s="35"/>
-      <c r="I18" s="36"/>
-      <c r="J18" s="37"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="20"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="25"/>
+      <c r="J18" s="26"/>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
@@ -974,36 +974,36 @@
       </c>
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B23" s="38" t="s">
+      <c r="B23" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C23" s="39" t="s">
+      <c r="C23" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D23" s="39" t="s">
+      <c r="D23" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E23" s="40" t="s">
+      <c r="E23" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="F23" s="41" t="s">
+      <c r="F23" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="G23" s="41" t="s">
+      <c r="G23" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="H23" s="42" t="s">
+      <c r="H23" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="I23" s="41"/>
+      <c r="I23" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="B15:D17"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="F16:G18"/>
-    <mergeCell ref="I16:J18"/>
+    <mergeCell ref="B2:E3"/>
+    <mergeCell ref="F2:G3"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B8:D8"/>
     <mergeCell ref="B10:D10"/>
     <mergeCell ref="B11:D11"/>
     <mergeCell ref="H6:L6"/>
@@ -1012,12 +1012,12 @@
     <mergeCell ref="H9:L9"/>
     <mergeCell ref="H10:L10"/>
     <mergeCell ref="H11:L11"/>
-    <mergeCell ref="B2:E3"/>
-    <mergeCell ref="F2:G3"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B8:D8"/>
     <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B15:D17"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="F16:G18"/>
+    <mergeCell ref="I16:J18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>